<commit_message>
Refactored code - removed all static methods.
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\Programming\Java\viko\2Dgame\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Player</t>
   </si>
@@ -119,12 +119,16 @@
   </si>
   <si>
     <t>BOBAS</t>
+  </si>
+  <si>
+    <t>UGNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -470,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
@@ -478,7 +482,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,6 +792,14 @@
       </c>
       <c r="B39">
         <v>200</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="n">
+        <v>200.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added restart game functionality.
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Player</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>UGNE</t>
+  </si>
+  <si>
+    <t>VITALIJUS</t>
+  </si>
+  <si>
+    <t>LAJA</t>
   </si>
 </sst>
 </file>
@@ -474,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
@@ -802,6 +808,38 @@
         <v>200.0</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="n">
+        <v>200.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished game. Refactored variables with get and set methods. Styled top 100 players HTML.
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\Programming\Java\viko\2Dgame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96437A3-76B1-449E-B7BE-8AA8B7108D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A34FF-F2D5-44F2-86CE-FBA8F15FE3C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Player</t>
   </si>
@@ -88,9 +88,6 @@
     <t>NERIJUS</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>NIKOLA</t>
   </si>
   <si>
@@ -128,13 +125,27 @@
   </si>
   <si>
     <t>LAJA</t>
+  </si>
+  <si>
+    <t>ROMAS</t>
+  </si>
+  <si>
+    <t>ERNESTAS</t>
+  </si>
+  <si>
+    <t>ONA</t>
+  </si>
+  <si>
+    <t>DOMANTAS</t>
+  </si>
+  <si>
+    <t>ULA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,15 +491,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +688,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>200</v>
@@ -682,7 +696,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>200</v>
@@ -690,7 +704,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>200</v>
@@ -698,7 +712,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>200</v>
@@ -706,7 +720,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>200</v>
@@ -714,7 +728,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>200</v>
@@ -722,7 +736,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>200</v>
@@ -730,15 +744,15 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B31">
-        <v>200</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>200</v>
@@ -746,7 +760,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>200</v>
@@ -754,7 +768,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>200</v>
@@ -762,7 +776,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>200</v>
@@ -770,7 +784,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>200</v>
@@ -778,7 +792,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B37">
         <v>200</v>
@@ -786,58 +800,34 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>1200</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>200</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" t="n">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" t="n">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" t="n">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" t="n">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" t="n">
-        <v>200.0</v>
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>